<commit_message>
everything but email report
</commit_message>
<xml_diff>
--- a/os_sales_report.xlsx
+++ b/os_sales_report.xlsx
@@ -12,13 +12,13 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="data-20201222-182650.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="OS OPRs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"data-20201222-182650.csv"</definedName>
   </definedNames>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="152511" iterate="1"/>
   <webPublishing css="0" allowPng="1" codePage="0"/>
 </workbook>
 </file>
@@ -409,14 +409,14 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="29.5703125" customWidth="1"/>
@@ -435,10 +435,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>